<commit_message>
Attendance up to date as of 10/04/2021. Week 6 and Week 7 time sheet
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week6.xlsx
+++ b/Admin/Gaby/TimeSheet_Week6.xlsx
@@ -369,10 +369,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -493,10 +493,12 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="11"/>
+      <c r="H7" s="11" t="n">
+        <v>2</v>
+      </c>
       <c r="I7" s="13" t="n">
         <f aca="false">SUM(B7:H7)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J7" s="9"/>
     </row>
@@ -563,12 +565,14 @@
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="F11" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="G11" s="12"/>
       <c r="H11" s="11"/>
       <c r="I11" s="13" t="n">
         <f aca="false">SUM(B11:H11)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11" s="9"/>
     </row>
@@ -582,10 +586,12 @@
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="11"/>
+      <c r="H12" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I12" s="13" t="n">
         <f aca="false">SUM(B12:H12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="9"/>
     </row>
@@ -630,7 +636,7 @@
       </c>
       <c r="F14" s="13" t="n">
         <f aca="false">SUM(F6:F13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="13" t="n">
         <f aca="false">SUM(G6:G13)</f>
@@ -638,11 +644,11 @@
       </c>
       <c r="H14" s="13" t="n">
         <f aca="false">SUM(H6:H13)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I14" s="13" t="n">
         <f aca="false">SUM(I6:I13)</f>
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>